<commit_message>
added better functionality. can now run as many rotations as you want in 1 prompt
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -556,6 +556,141 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>owen</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>ethan</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>sdr</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>james</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>eric</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>zach</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>serge</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>george</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>jason</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>oscar</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>joey</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>wilfredo</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>chris</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>kamy</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>owen</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>ethan</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>sdr</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>james</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>eric</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>zach</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>serge</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>george</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>jason</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>oscar</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>joey</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>